<commit_message>
Add better contactors snubbers
</commit_message>
<xml_diff>
--- a/docs/BOM.xlsx
+++ b/docs/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmatt\Documents\anchor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A294A35-AD81-435B-B0A8-49E681524F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2157D4D5-6706-459C-956D-721DA830B48F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13800" yWindow="5550" windowWidth="18045" windowHeight="14715" xr2:uid="{50EE7513-1BEB-47B5-BCED-D1BDEC199D6D}"/>
+    <workbookView xWindow="11850" yWindow="5205" windowWidth="18045" windowHeight="14715" xr2:uid="{50EE7513-1BEB-47B5-BCED-D1BDEC199D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Category</t>
   </si>
@@ -82,6 +82,21 @@
   </si>
   <si>
     <t>G5LE-14-DC5 SPDT 10A Relay</t>
+  </si>
+  <si>
+    <t>Murrelektronik</t>
+  </si>
+  <si>
+    <t>https://www.automationdirect.com/adc/shopping/catalog/power_products_(electrical)/surge_suppression_devices/universal_surge_suppressors/26183</t>
+  </si>
+  <si>
+    <t>https://www.automationdirect.com/adc/shopping/catalog/power_products_(electrical)/surge_suppression_devices/universal_surge_suppressors/26051</t>
+  </si>
+  <si>
+    <t>110-250 VAC 0-60 Hz Varistor Module</t>
+  </si>
+  <si>
+    <t>12-30 VDC Diode-Zender Suppressor Module</t>
   </si>
 </sst>
 </file>
@@ -89,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -134,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -143,10 +158,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -155,6 +170,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,20 +497,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D6B4AC3-A139-4AC1-AF30-46E7B9A94A1B}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="39" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
-    <col min="6" max="7" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="12" customWidth="1"/>
     <col min="8" max="8" width="0.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
   </cols>
@@ -506,7 +535,7 @@
       <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="7"/>
@@ -581,11 +610,12 @@
       <c r="F3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="4">
         <v>1.68</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="1">
+        <f t="shared" ref="I3:I5" si="0">_xlfn.CEILING.MATH(E3/F3)</f>
         <v>1</v>
       </c>
       <c r="J3" s="4">
@@ -598,6 +628,80 @@
       </c>
       <c r="L3" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="1">
+        <v>26183</v>
+      </c>
+      <c r="E4" s="8">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11">
+        <v>8.25</v>
+      </c>
+      <c r="H4" s="9"/>
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J4" s="4">
+        <f>E4*(G4/F4)</f>
+        <v>8.25</v>
+      </c>
+      <c r="K4" s="4">
+        <f>I4*G4</f>
+        <v>8.25</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1">
+        <v>26051</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>8</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J5" s="4">
+        <f>E5*(G5/F5)</f>
+        <v>24</v>
+      </c>
+      <c r="K5" s="4">
+        <f>I5*G5</f>
+        <v>24</v>
+      </c>
+      <c r="L5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>